<commit_message>
clean and orgnize the files and code. write how to run the code to porduce the schedule of the interivews
</commit_message>
<xml_diff>
--- a/company_list.xlsx
+++ b/company_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aseelalshohatee/Documents/tolexcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACB6473-4367-2641-864A-BFEA0F6F2D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E7426A-AB99-4F4C-805B-487DA86FAEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apple" sheetId="4" r:id="rId1"/>
@@ -21,28 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t xml:space="preserve">Fname </t>
-  </si>
-  <si>
-    <t>Lname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time </t>
-  </si>
-  <si>
-    <t>Ashlyn</t>
-  </si>
-  <si>
-    <t>Reich</t>
-  </si>
-  <si>
-    <t>Aurelio</t>
-  </si>
-  <si>
-    <t>Molina</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Avril</t>
   </si>
@@ -68,15 +47,6 @@
     <t>Willett</t>
   </si>
   <si>
-    <t xml:space="preserve">first name </t>
-  </si>
-  <si>
-    <t>last name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time </t>
-  </si>
-  <si>
     <t>Saran</t>
   </si>
   <si>
@@ -105,6 +75,15 @@
   </si>
   <si>
     <t>Forbes</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>fname</t>
   </si>
 </sst>
 </file>
@@ -370,79 +349,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C22B45-5B37-A442-B804-28F32B1F72BB}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -451,78 +420,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D1FD71-7706-6643-AD4B-17B85B88AF51}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>